<commit_message>
Add dynamic data & Refactor
</commit_message>
<xml_diff>
--- a/src/test/java/data/user_info.xlsx
+++ b/src/test/java/data/user_info.xlsx
@@ -20,18 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">ehab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaaban</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">captain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100403457</t>
   </si>
   <si>
     <t xml:space="preserve">asdaf@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">John</t>
+    <t xml:space="preserve">Ad455111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hArY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100403123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddddD454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john</t>
   </si>
   <si>
     <t xml:space="preserve">wick</t>
@@ -40,13 +58,46 @@
     <t xml:space="preserve">ha_ffff@yahoo.com</t>
   </si>
   <si>
-    <t xml:space="preserve">jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jhagdf@hola.com</t>
+    <t xml:space="preserve">Magdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01200856942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33333333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01200856900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ha@asdcom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddddZZ454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pencil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01200856800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hfgcompany.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddddZZ450</t>
   </si>
 </sst>
 </file>
@@ -159,14 +210,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.3"/>
   </cols>
   <sheetData>
@@ -177,64 +229,126 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>12185451</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>123456</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>88888888</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>444444</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>444444</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>2222222</v>
+        <v>88888888</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1111111</v>
+        <v>444444</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>2222222</v>
+        <v>444444</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>444444</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="asdaf@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="ha_ffff@yahoo.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="jhagdf@hola.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="asdaf@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId3" display="ha_ffff@yahoo.com"/>
+    <hyperlink ref="D4" r:id="rId4" display="ha_ffff@yahoo.com"/>
+    <hyperlink ref="D5" r:id="rId5" display="ha@asdcom"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>